<commit_message>
Configuration de GLPI et de l annuraire LDAP
</commit_message>
<xml_diff>
--- a/Documentation/2023.05.02_Nonnenmacher_Enzo_Planification initiale.xlsx
+++ b/Documentation/2023.05.02_Nonnenmacher_Enzo_Planification initiale.xlsx
@@ -863,15 +863,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB7B7B7"/>
       </left>
@@ -1385,11 +1376,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1560,15 +1560,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="25" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1591,7 +1587,7 @@
     <xf numFmtId="0" fontId="29" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="28" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1604,76 +1600,76 @@
     <xf numFmtId="0" fontId="28" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="21" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1690,7 +1686,7 @@
     <xf numFmtId="0" fontId="28" fillId="29" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1717,7 +1713,7 @@
     <xf numFmtId="0" fontId="33" fillId="26" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="27" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1741,15 +1737,15 @@
     <xf numFmtId="166" fontId="25" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1763,41 +1759,44 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="28" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1824,105 +1823,38 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="22" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="22" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="22" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="17" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="17" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="17" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="17" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="17" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="17" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="17" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1941,7 +1873,74 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2229,7 +2228,7 @@
   <dimension ref="A1:BL44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -2328,35 +2327,35 @@
     </row>
     <row r="2" spans="1:64" ht="27" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="197" t="s">
+      <c r="B2" s="173" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="196"/>
-      <c r="O2" s="196"/>
-      <c r="P2" s="196"/>
-      <c r="Q2" s="196"/>
-      <c r="R2" s="196"/>
-      <c r="S2" s="196"/>
-      <c r="T2" s="196"/>
-      <c r="U2" s="196"/>
-      <c r="V2" s="196"/>
-      <c r="W2" s="196"/>
-      <c r="X2" s="196"/>
-      <c r="Y2" s="196"/>
-      <c r="Z2" s="196"/>
-      <c r="AA2" s="196"/>
-      <c r="AB2" s="196"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="171"/>
+      <c r="J2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
+      <c r="M2" s="172"/>
+      <c r="N2" s="172"/>
+      <c r="O2" s="172"/>
+      <c r="P2" s="172"/>
+      <c r="Q2" s="172"/>
+      <c r="R2" s="172"/>
+      <c r="S2" s="172"/>
+      <c r="T2" s="172"/>
+      <c r="U2" s="172"/>
+      <c r="V2" s="172"/>
+      <c r="W2" s="172"/>
+      <c r="X2" s="172"/>
+      <c r="Y2" s="172"/>
+      <c r="Z2" s="172"/>
+      <c r="AA2" s="172"/>
+      <c r="AB2" s="172"/>
       <c r="AC2" s="10"/>
       <c r="AD2" s="10"/>
       <c r="AE2" s="10"/>
@@ -2462,37 +2461,37 @@
     </row>
     <row r="4" spans="1:64" ht="22.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="175" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="200"/>
-      <c r="D4" s="201" t="s">
+      <c r="C4" s="176"/>
+      <c r="D4" s="177" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="200"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="200"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="176"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="65" t="s">
+      <c r="I4" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="62" t="s">
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="202" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="64"/>
+      <c r="O4" s="202"/>
+      <c r="P4" s="202"/>
+      <c r="Q4" s="202"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="63"/>
+      <c r="X4" s="63"/>
       <c r="Y4" s="16"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
@@ -2536,36 +2535,36 @@
     </row>
     <row r="5" spans="1:64" ht="21" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="202" t="s">
+      <c r="C5" s="176"/>
+      <c r="D5" s="178" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="200"/>
-      <c r="F5" s="200"/>
-      <c r="G5" s="200"/>
+      <c r="E5" s="176"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="176"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="176" t="s">
+      <c r="I5" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="176"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="177">
+      <c r="J5" s="194"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="195">
         <v>45048</v>
       </c>
-      <c r="M5" s="177"/>
-      <c r="N5" s="177"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="64"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
+      <c r="M5" s="195"/>
+      <c r="N5" s="195"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
       <c r="X5" s="18"/>
       <c r="Y5" s="16"/>
       <c r="Z5" s="1"/>
@@ -2742,166 +2741,166 @@
     </row>
     <row r="8" spans="1:64" ht="17.25" customHeight="1">
       <c r="A8" s="23"/>
-      <c r="B8" s="193" t="s">
+      <c r="B8" s="166" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="193" t="s">
+      <c r="C8" s="166" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="193" t="s">
+      <c r="D8" s="166" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="193" t="s">
+      <c r="E8" s="166" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="193" t="s">
+      <c r="F8" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="193" t="s">
+      <c r="G8" s="166" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="193" t="s">
+      <c r="H8" s="166" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="183" t="s">
+      <c r="I8" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="184"/>
-      <c r="K8" s="184"/>
-      <c r="L8" s="184"/>
-      <c r="M8" s="184"/>
-      <c r="N8" s="184"/>
-      <c r="O8" s="184"/>
-      <c r="P8" s="184"/>
-      <c r="Q8" s="184"/>
-      <c r="R8" s="184"/>
-      <c r="S8" s="184"/>
-      <c r="T8" s="184"/>
-      <c r="U8" s="184"/>
-      <c r="V8" s="184"/>
-      <c r="W8" s="184"/>
-      <c r="X8" s="184"/>
-      <c r="Y8" s="184"/>
-      <c r="Z8" s="184"/>
-      <c r="AA8" s="184"/>
+      <c r="J8" s="200"/>
+      <c r="K8" s="200"/>
+      <c r="L8" s="200"/>
+      <c r="M8" s="200"/>
+      <c r="N8" s="200"/>
+      <c r="O8" s="200"/>
+      <c r="P8" s="200"/>
+      <c r="Q8" s="200"/>
+      <c r="R8" s="200"/>
+      <c r="S8" s="200"/>
+      <c r="T8" s="200"/>
+      <c r="U8" s="200"/>
+      <c r="V8" s="200"/>
+      <c r="W8" s="200"/>
+      <c r="X8" s="200"/>
+      <c r="Y8" s="200"/>
+      <c r="Z8" s="200"/>
+      <c r="AA8" s="200"/>
       <c r="AB8" s="47"/>
-      <c r="AH8" s="191"/>
-      <c r="AI8" s="190"/>
-      <c r="AJ8" s="190"/>
-      <c r="AK8" s="190"/>
-      <c r="AL8" s="190"/>
-      <c r="AM8" s="190"/>
-      <c r="AN8" s="190"/>
-      <c r="AO8" s="190"/>
-      <c r="AP8" s="190"/>
-      <c r="AQ8" s="190"/>
-      <c r="AR8" s="190"/>
-      <c r="AS8" s="190"/>
-      <c r="AT8" s="190"/>
-      <c r="AU8" s="190"/>
-      <c r="AV8" s="190"/>
-      <c r="AW8" s="189"/>
-      <c r="AX8" s="190"/>
-      <c r="AY8" s="190"/>
-      <c r="AZ8" s="190"/>
-      <c r="BA8" s="190"/>
-      <c r="BB8" s="190"/>
-      <c r="BC8" s="190"/>
-      <c r="BD8" s="190"/>
-      <c r="BE8" s="190"/>
-      <c r="BF8" s="190"/>
-      <c r="BG8" s="190"/>
-      <c r="BH8" s="190"/>
-      <c r="BI8" s="190"/>
-      <c r="BJ8" s="190"/>
-      <c r="BK8" s="179"/>
+      <c r="AH8" s="183"/>
+      <c r="AI8" s="182"/>
+      <c r="AJ8" s="182"/>
+      <c r="AK8" s="182"/>
+      <c r="AL8" s="182"/>
+      <c r="AM8" s="182"/>
+      <c r="AN8" s="182"/>
+      <c r="AO8" s="182"/>
+      <c r="AP8" s="182"/>
+      <c r="AQ8" s="182"/>
+      <c r="AR8" s="182"/>
+      <c r="AS8" s="182"/>
+      <c r="AT8" s="182"/>
+      <c r="AU8" s="182"/>
+      <c r="AV8" s="182"/>
+      <c r="AW8" s="181"/>
+      <c r="AX8" s="182"/>
+      <c r="AY8" s="182"/>
+      <c r="AZ8" s="182"/>
+      <c r="BA8" s="182"/>
+      <c r="BB8" s="182"/>
+      <c r="BC8" s="182"/>
+      <c r="BD8" s="182"/>
+      <c r="BE8" s="182"/>
+      <c r="BF8" s="182"/>
+      <c r="BG8" s="182"/>
+      <c r="BH8" s="182"/>
+      <c r="BI8" s="182"/>
+      <c r="BJ8" s="182"/>
+      <c r="BK8" s="180"/>
       <c r="BL8" s="20"/>
     </row>
     <row r="9" spans="1:64" ht="17.25" customHeight="1">
       <c r="A9" s="24"/>
-      <c r="B9" s="194"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
-      <c r="I9" s="186" t="s">
+      <c r="B9" s="167"/>
+      <c r="C9" s="167"/>
+      <c r="D9" s="167"/>
+      <c r="E9" s="167"/>
+      <c r="F9" s="167"/>
+      <c r="G9" s="167"/>
+      <c r="H9" s="167"/>
+      <c r="I9" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="187"/>
-      <c r="K9" s="188"/>
-      <c r="L9" s="187" t="s">
+      <c r="J9" s="168"/>
+      <c r="K9" s="170"/>
+      <c r="L9" s="168" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="187"/>
-      <c r="N9" s="187"/>
-      <c r="O9" s="187"/>
-      <c r="P9" s="186" t="s">
+      <c r="M9" s="168"/>
+      <c r="N9" s="168"/>
+      <c r="O9" s="168"/>
+      <c r="P9" s="169" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="187"/>
-      <c r="R9" s="187"/>
-      <c r="S9" s="188"/>
-      <c r="T9" s="180" t="s">
+      <c r="Q9" s="168"/>
+      <c r="R9" s="168"/>
+      <c r="S9" s="170"/>
+      <c r="T9" s="196" t="s">
         <v>14</v>
       </c>
-      <c r="U9" s="181"/>
-      <c r="V9" s="181"/>
-      <c r="W9" s="181"/>
-      <c r="X9" s="180" t="s">
+      <c r="U9" s="197"/>
+      <c r="V9" s="197"/>
+      <c r="W9" s="197"/>
+      <c r="X9" s="196" t="s">
         <v>15</v>
       </c>
-      <c r="Y9" s="181"/>
-      <c r="Z9" s="181"/>
-      <c r="AA9" s="182"/>
+      <c r="Y9" s="197"/>
+      <c r="Z9" s="197"/>
+      <c r="AA9" s="198"/>
       <c r="AB9" s="48"/>
-      <c r="AC9" s="185"/>
-      <c r="AD9" s="179"/>
-      <c r="AE9" s="179"/>
-      <c r="AF9" s="179"/>
-      <c r="AG9" s="179"/>
-      <c r="AH9" s="192"/>
-      <c r="AI9" s="179"/>
-      <c r="AJ9" s="179"/>
-      <c r="AK9" s="179"/>
-      <c r="AL9" s="179"/>
-      <c r="AM9" s="192"/>
-      <c r="AN9" s="179"/>
-      <c r="AO9" s="179"/>
-      <c r="AP9" s="179"/>
-      <c r="AQ9" s="179"/>
-      <c r="AR9" s="192"/>
-      <c r="AS9" s="179"/>
-      <c r="AT9" s="179"/>
-      <c r="AU9" s="179"/>
-      <c r="AV9" s="179"/>
-      <c r="AW9" s="178"/>
-      <c r="AX9" s="179"/>
-      <c r="AY9" s="179"/>
-      <c r="AZ9" s="179"/>
-      <c r="BA9" s="179"/>
-      <c r="BB9" s="178"/>
-      <c r="BC9" s="179"/>
-      <c r="BD9" s="179"/>
-      <c r="BE9" s="179"/>
-      <c r="BF9" s="179"/>
-      <c r="BG9" s="178"/>
-      <c r="BH9" s="179"/>
-      <c r="BI9" s="179"/>
-      <c r="BJ9" s="179"/>
-      <c r="BK9" s="179"/>
+      <c r="AC9" s="201"/>
+      <c r="AD9" s="180"/>
+      <c r="AE9" s="180"/>
+      <c r="AF9" s="180"/>
+      <c r="AG9" s="180"/>
+      <c r="AH9" s="184"/>
+      <c r="AI9" s="180"/>
+      <c r="AJ9" s="180"/>
+      <c r="AK9" s="180"/>
+      <c r="AL9" s="180"/>
+      <c r="AM9" s="184"/>
+      <c r="AN9" s="180"/>
+      <c r="AO9" s="180"/>
+      <c r="AP9" s="180"/>
+      <c r="AQ9" s="180"/>
+      <c r="AR9" s="184"/>
+      <c r="AS9" s="180"/>
+      <c r="AT9" s="180"/>
+      <c r="AU9" s="180"/>
+      <c r="AV9" s="180"/>
+      <c r="AW9" s="179"/>
+      <c r="AX9" s="180"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="180"/>
+      <c r="BB9" s="179"/>
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="180"/>
+      <c r="BG9" s="179"/>
+      <c r="BH9" s="180"/>
+      <c r="BI9" s="180"/>
+      <c r="BJ9" s="180"/>
+      <c r="BK9" s="180"/>
       <c r="BL9" s="24"/>
     </row>
     <row r="10" spans="1:64" ht="17.25" customHeight="1">
       <c r="A10" s="25"/>
-      <c r="B10" s="194"/>
-      <c r="C10" s="194"/>
-      <c r="D10" s="194"/>
-      <c r="E10" s="194"/>
-      <c r="F10" s="194"/>
-      <c r="G10" s="194"/>
-      <c r="H10" s="194"/>
+      <c r="B10" s="167"/>
+      <c r="C10" s="167"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="167"/>
+      <c r="F10" s="167"/>
+      <c r="G10" s="167"/>
+      <c r="H10" s="167"/>
       <c r="I10" s="26" t="s">
         <v>17</v>
       </c>
@@ -2999,47 +2998,47 @@
     </row>
     <row r="11" spans="1:64" ht="21" customHeight="1">
       <c r="A11" s="20"/>
-      <c r="B11" s="121">
+      <c r="B11" s="119">
         <v>1</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="123"/>
-      <c r="E11" s="124">
+      <c r="D11" s="121"/>
+      <c r="E11" s="122">
         <v>45048</v>
       </c>
-      <c r="F11" s="124">
+      <c r="F11" s="122">
         <v>45051</v>
       </c>
-      <c r="G11" s="125">
+      <c r="G11" s="123">
         <f>SUM(G12:G15)</f>
         <v>7</v>
       </c>
-      <c r="H11" s="123"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="167" t="s">
+      <c r="H11" s="121"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="71"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="185" t="s">
         <v>54</v>
       </c>
-      <c r="S11" s="168"/>
-      <c r="T11" s="73"/>
-      <c r="U11" s="73"/>
-      <c r="V11" s="73"/>
-      <c r="W11" s="73"/>
-      <c r="X11" s="173" t="s">
+      <c r="S11" s="186"/>
+      <c r="T11" s="71"/>
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71"/>
+      <c r="X11" s="191" t="s">
         <v>54</v>
       </c>
-      <c r="Y11" s="73"/>
-      <c r="Z11" s="73"/>
-      <c r="AA11" s="74"/>
+      <c r="Y11" s="71"/>
+      <c r="Z11" s="71"/>
+      <c r="AA11" s="72"/>
       <c r="AB11" s="41"/>
       <c r="AC11" s="41"/>
       <c r="AD11" s="41"/>
@@ -3098,32 +3097,32 @@
       <c r="G12" s="56">
         <v>2</v>
       </c>
-      <c r="H12" s="126">
+      <c r="H12" s="124">
         <v>1</v>
       </c>
-      <c r="I12" s="71" t="s">
+      <c r="I12" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="87" t="s">
+      <c r="J12" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="K12" s="112"/>
-      <c r="L12" s="127"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="128"/>
-      <c r="R12" s="169"/>
-      <c r="S12" s="170"/>
-      <c r="T12" s="152"/>
-      <c r="U12" s="153"/>
-      <c r="V12" s="153"/>
-      <c r="W12" s="154"/>
-      <c r="X12" s="174"/>
-      <c r="Y12" s="161"/>
-      <c r="Z12" s="162"/>
-      <c r="AA12" s="162"/>
+      <c r="K12" s="110"/>
+      <c r="L12" s="125"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="126"/>
+      <c r="R12" s="187"/>
+      <c r="S12" s="188"/>
+      <c r="T12" s="150"/>
+      <c r="U12" s="151"/>
+      <c r="V12" s="151"/>
+      <c r="W12" s="152"/>
+      <c r="X12" s="192"/>
+      <c r="Y12" s="159"/>
+      <c r="Z12" s="160"/>
+      <c r="AA12" s="160"/>
       <c r="AB12" s="49"/>
       <c r="AC12" s="42"/>
       <c r="AD12" s="42"/>
@@ -3162,7 +3161,7 @@
       <c r="BK12" s="42"/>
       <c r="BL12" s="30"/>
     </row>
-    <row r="13" spans="1:64" s="63" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1">
+    <row r="13" spans="1:64" s="62" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
       <c r="B13" s="53">
         <v>44958</v>
@@ -3182,30 +3181,30 @@
       <c r="G13" s="56">
         <v>1</v>
       </c>
-      <c r="H13" s="126">
+      <c r="H13" s="124">
         <v>0</v>
       </c>
-      <c r="I13" s="129"/>
-      <c r="J13" s="97" t="s">
+      <c r="I13" s="127"/>
+      <c r="J13" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="108"/>
-      <c r="L13" s="130"/>
-      <c r="M13" s="99"/>
-      <c r="N13" s="99"/>
-      <c r="O13" s="99"/>
-      <c r="P13" s="99"/>
-      <c r="Q13" s="131"/>
-      <c r="R13" s="169"/>
-      <c r="S13" s="170"/>
-      <c r="T13" s="155"/>
-      <c r="U13" s="156"/>
-      <c r="V13" s="156"/>
-      <c r="W13" s="157"/>
-      <c r="X13" s="174"/>
-      <c r="Y13" s="163"/>
-      <c r="Z13" s="164"/>
-      <c r="AA13" s="164"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="128"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="97"/>
+      <c r="P13" s="97"/>
+      <c r="Q13" s="129"/>
+      <c r="R13" s="187"/>
+      <c r="S13" s="188"/>
+      <c r="T13" s="153"/>
+      <c r="U13" s="154"/>
+      <c r="V13" s="154"/>
+      <c r="W13" s="155"/>
+      <c r="X13" s="192"/>
+      <c r="Y13" s="161"/>
+      <c r="Z13" s="162"/>
+      <c r="AA13" s="162"/>
       <c r="AB13" s="49"/>
       <c r="AC13" s="42"/>
       <c r="AD13" s="42"/>
@@ -3244,7 +3243,7 @@
       <c r="BK13" s="42"/>
       <c r="BL13" s="30"/>
     </row>
-    <row r="14" spans="1:64" s="63" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1">
+    <row r="14" spans="1:64" s="62" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
       <c r="B14" s="53">
         <v>44986</v>
@@ -3264,32 +3263,32 @@
       <c r="G14" s="56">
         <v>2</v>
       </c>
-      <c r="H14" s="67">
+      <c r="H14" s="65">
         <v>0</v>
       </c>
-      <c r="I14" s="129"/>
-      <c r="J14" s="97" t="s">
+      <c r="I14" s="127"/>
+      <c r="J14" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="97" t="s">
+      <c r="K14" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="L14" s="130"/>
-      <c r="M14" s="99"/>
-      <c r="N14" s="99"/>
-      <c r="O14" s="99"/>
-      <c r="P14" s="99"/>
-      <c r="Q14" s="131"/>
-      <c r="R14" s="169"/>
-      <c r="S14" s="170"/>
-      <c r="T14" s="158"/>
-      <c r="U14" s="159"/>
-      <c r="V14" s="159"/>
-      <c r="W14" s="160"/>
-      <c r="X14" s="174"/>
-      <c r="Y14" s="165"/>
-      <c r="Z14" s="166"/>
-      <c r="AA14" s="166"/>
+      <c r="L14" s="128"/>
+      <c r="M14" s="97"/>
+      <c r="N14" s="97"/>
+      <c r="O14" s="97"/>
+      <c r="P14" s="97"/>
+      <c r="Q14" s="129"/>
+      <c r="R14" s="187"/>
+      <c r="S14" s="188"/>
+      <c r="T14" s="156"/>
+      <c r="U14" s="157"/>
+      <c r="V14" s="157"/>
+      <c r="W14" s="158"/>
+      <c r="X14" s="192"/>
+      <c r="Y14" s="163"/>
+      <c r="Z14" s="164"/>
+      <c r="AA14" s="164"/>
       <c r="AB14" s="49"/>
       <c r="AC14" s="42"/>
       <c r="AD14" s="42"/>
@@ -3348,32 +3347,32 @@
       <c r="G15" s="56">
         <v>2</v>
       </c>
-      <c r="H15" s="67">
+      <c r="H15" s="65">
         <v>0</v>
       </c>
-      <c r="I15" s="75"/>
-      <c r="J15" s="76" t="s">
+      <c r="I15" s="73"/>
+      <c r="J15" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="K15" s="134" t="s">
+      <c r="K15" s="132" t="s">
         <v>58</v>
       </c>
-      <c r="L15" s="78"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="80"/>
-      <c r="R15" s="169"/>
-      <c r="S15" s="170"/>
-      <c r="T15" s="81"/>
-      <c r="U15" s="77"/>
-      <c r="V15" s="77"/>
-      <c r="W15" s="80"/>
-      <c r="X15" s="174"/>
-      <c r="Y15" s="82"/>
-      <c r="Z15" s="83"/>
-      <c r="AA15" s="83"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="77"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="77"/>
+      <c r="P15" s="77"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="187"/>
+      <c r="S15" s="188"/>
+      <c r="T15" s="79"/>
+      <c r="U15" s="75"/>
+      <c r="V15" s="75"/>
+      <c r="W15" s="78"/>
+      <c r="X15" s="192"/>
+      <c r="Y15" s="80"/>
+      <c r="Z15" s="81"/>
+      <c r="AA15" s="81"/>
       <c r="AB15" s="49"/>
       <c r="AC15" s="42"/>
       <c r="AD15" s="42"/>
@@ -3421,36 +3420,36 @@
         <v>31</v>
       </c>
       <c r="D16" s="29"/>
-      <c r="E16" s="68">
+      <c r="E16" s="66">
         <v>45054</v>
       </c>
-      <c r="F16" s="68">
+      <c r="F16" s="66">
         <v>45069</v>
       </c>
-      <c r="G16" s="69">
+      <c r="G16" s="67">
         <f>SUM(G17:G26)</f>
         <v>13</v>
       </c>
       <c r="H16" s="29"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="85"/>
-      <c r="K16" s="85"/>
-      <c r="L16" s="85"/>
-      <c r="M16" s="85"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="85"/>
-      <c r="P16" s="85"/>
-      <c r="Q16" s="85"/>
-      <c r="R16" s="169"/>
-      <c r="S16" s="170"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="73"/>
-      <c r="V16" s="73"/>
-      <c r="W16" s="73"/>
-      <c r="X16" s="174"/>
-      <c r="Y16" s="73"/>
-      <c r="Z16" s="73"/>
-      <c r="AA16" s="74"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="83"/>
+      <c r="M16" s="83"/>
+      <c r="N16" s="83"/>
+      <c r="O16" s="83"/>
+      <c r="P16" s="83"/>
+      <c r="Q16" s="83"/>
+      <c r="R16" s="187"/>
+      <c r="S16" s="188"/>
+      <c r="T16" s="71"/>
+      <c r="U16" s="71"/>
+      <c r="V16" s="71"/>
+      <c r="W16" s="71"/>
+      <c r="X16" s="192"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="72"/>
       <c r="AB16" s="51"/>
       <c r="AC16" s="42"/>
       <c r="AD16" s="42"/>
@@ -3512,29 +3511,29 @@
       <c r="H17" s="35">
         <v>0</v>
       </c>
-      <c r="I17" s="86"/>
-      <c r="J17" s="112" t="s">
+      <c r="I17" s="84"/>
+      <c r="J17" s="110" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="135"/>
-      <c r="L17" s="87" t="s">
+      <c r="K17" s="133"/>
+      <c r="L17" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="M17" s="89"/>
-      <c r="N17" s="89"/>
-      <c r="O17" s="89"/>
-      <c r="P17" s="89"/>
-      <c r="Q17" s="128"/>
-      <c r="R17" s="169"/>
-      <c r="S17" s="170"/>
-      <c r="T17" s="91"/>
-      <c r="U17" s="92"/>
-      <c r="V17" s="92"/>
-      <c r="W17" s="93"/>
-      <c r="X17" s="174"/>
-      <c r="Y17" s="94"/>
-      <c r="Z17" s="95"/>
-      <c r="AA17" s="95"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="87"/>
+      <c r="P17" s="87"/>
+      <c r="Q17" s="126"/>
+      <c r="R17" s="187"/>
+      <c r="S17" s="188"/>
+      <c r="T17" s="89"/>
+      <c r="U17" s="90"/>
+      <c r="V17" s="90"/>
+      <c r="W17" s="91"/>
+      <c r="X17" s="192"/>
+      <c r="Y17" s="92"/>
+      <c r="Z17" s="93"/>
+      <c r="AA17" s="93"/>
       <c r="AB17" s="51"/>
       <c r="AC17" s="42"/>
       <c r="AD17" s="42"/>
@@ -3596,29 +3595,29 @@
       <c r="H18" s="35">
         <v>0</v>
       </c>
-      <c r="I18" s="96"/>
-      <c r="J18" s="108" t="s">
+      <c r="I18" s="94"/>
+      <c r="J18" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="K18" s="136"/>
-      <c r="L18" s="97" t="s">
+      <c r="K18" s="134"/>
+      <c r="L18" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="M18" s="99"/>
-      <c r="N18" s="99"/>
-      <c r="O18" s="99"/>
-      <c r="P18" s="99"/>
-      <c r="Q18" s="131"/>
-      <c r="R18" s="169"/>
-      <c r="S18" s="170"/>
-      <c r="T18" s="101"/>
-      <c r="U18" s="102"/>
-      <c r="V18" s="102"/>
-      <c r="W18" s="100"/>
-      <c r="X18" s="174"/>
-      <c r="Y18" s="103"/>
-      <c r="Z18" s="104"/>
-      <c r="AA18" s="105"/>
+      <c r="M18" s="97"/>
+      <c r="N18" s="97"/>
+      <c r="O18" s="97"/>
+      <c r="P18" s="97"/>
+      <c r="Q18" s="129"/>
+      <c r="R18" s="187"/>
+      <c r="S18" s="188"/>
+      <c r="T18" s="99"/>
+      <c r="U18" s="100"/>
+      <c r="V18" s="100"/>
+      <c r="W18" s="98"/>
+      <c r="X18" s="192"/>
+      <c r="Y18" s="101"/>
+      <c r="Z18" s="102"/>
+      <c r="AA18" s="103"/>
       <c r="AB18" s="51"/>
       <c r="AC18" s="42"/>
       <c r="AD18" s="42"/>
@@ -3680,29 +3679,29 @@
       <c r="H19" s="35">
         <v>0</v>
       </c>
-      <c r="I19" s="96"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="108" t="s">
+      <c r="I19" s="94"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="L19" s="97" t="s">
+      <c r="L19" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="M19" s="99"/>
-      <c r="N19" s="99"/>
-      <c r="O19" s="99"/>
-      <c r="P19" s="99"/>
-      <c r="Q19" s="131"/>
-      <c r="R19" s="169"/>
-      <c r="S19" s="170"/>
-      <c r="T19" s="101"/>
-      <c r="U19" s="102"/>
-      <c r="V19" s="102"/>
-      <c r="W19" s="100"/>
-      <c r="X19" s="174"/>
-      <c r="Y19" s="106"/>
-      <c r="Z19" s="107"/>
-      <c r="AA19" s="107"/>
+      <c r="M19" s="97"/>
+      <c r="N19" s="97"/>
+      <c r="O19" s="97"/>
+      <c r="P19" s="97"/>
+      <c r="Q19" s="129"/>
+      <c r="R19" s="187"/>
+      <c r="S19" s="188"/>
+      <c r="T19" s="99"/>
+      <c r="U19" s="100"/>
+      <c r="V19" s="100"/>
+      <c r="W19" s="98"/>
+      <c r="X19" s="192"/>
+      <c r="Y19" s="104"/>
+      <c r="Z19" s="105"/>
+      <c r="AA19" s="105"/>
       <c r="AB19" s="51"/>
       <c r="AC19" s="42"/>
       <c r="AD19" s="42"/>
@@ -3764,29 +3763,29 @@
       <c r="H20" s="35">
         <v>0</v>
       </c>
-      <c r="I20" s="96"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="108" t="s">
+      <c r="I20" s="94"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="L20" s="136"/>
-      <c r="M20" s="97" t="s">
+      <c r="L20" s="134"/>
+      <c r="M20" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="N20" s="99"/>
-      <c r="O20" s="99"/>
-      <c r="P20" s="99"/>
-      <c r="Q20" s="131"/>
-      <c r="R20" s="169"/>
-      <c r="S20" s="170"/>
-      <c r="T20" s="101"/>
-      <c r="U20" s="102"/>
-      <c r="V20" s="102"/>
-      <c r="W20" s="100"/>
-      <c r="X20" s="174"/>
-      <c r="Y20" s="106"/>
-      <c r="Z20" s="107"/>
-      <c r="AA20" s="107"/>
+      <c r="N20" s="97"/>
+      <c r="O20" s="97"/>
+      <c r="P20" s="97"/>
+      <c r="Q20" s="129"/>
+      <c r="R20" s="187"/>
+      <c r="S20" s="188"/>
+      <c r="T20" s="99"/>
+      <c r="U20" s="100"/>
+      <c r="V20" s="100"/>
+      <c r="W20" s="98"/>
+      <c r="X20" s="192"/>
+      <c r="Y20" s="104"/>
+      <c r="Z20" s="105"/>
+      <c r="AA20" s="105"/>
       <c r="AB20" s="51"/>
       <c r="AC20" s="42"/>
       <c r="AD20" s="42"/>
@@ -3848,29 +3847,29 @@
       <c r="H21" s="35">
         <v>0</v>
       </c>
-      <c r="I21" s="96"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="108" t="s">
+      <c r="I21" s="94"/>
+      <c r="J21" s="96"/>
+      <c r="K21" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="L21" s="136"/>
-      <c r="M21" s="97" t="s">
+      <c r="L21" s="134"/>
+      <c r="M21" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="N21" s="99"/>
-      <c r="O21" s="99"/>
-      <c r="P21" s="99"/>
-      <c r="Q21" s="131"/>
-      <c r="R21" s="169"/>
-      <c r="S21" s="170"/>
-      <c r="T21" s="101"/>
-      <c r="U21" s="102"/>
-      <c r="V21" s="102"/>
-      <c r="W21" s="100"/>
-      <c r="X21" s="174"/>
-      <c r="Y21" s="106"/>
-      <c r="Z21" s="107"/>
-      <c r="AA21" s="107"/>
+      <c r="N21" s="97"/>
+      <c r="O21" s="97"/>
+      <c r="P21" s="97"/>
+      <c r="Q21" s="129"/>
+      <c r="R21" s="187"/>
+      <c r="S21" s="188"/>
+      <c r="T21" s="99"/>
+      <c r="U21" s="100"/>
+      <c r="V21" s="100"/>
+      <c r="W21" s="98"/>
+      <c r="X21" s="192"/>
+      <c r="Y21" s="104"/>
+      <c r="Z21" s="105"/>
+      <c r="AA21" s="105"/>
       <c r="AB21" s="51"/>
       <c r="AC21" s="42"/>
       <c r="AD21" s="42"/>
@@ -3932,27 +3931,27 @@
       <c r="H22" s="35">
         <v>0</v>
       </c>
-      <c r="I22" s="96"/>
-      <c r="J22" s="98"/>
-      <c r="K22" s="98"/>
-      <c r="L22" s="136"/>
-      <c r="M22" s="97" t="s">
+      <c r="I22" s="94"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="134"/>
+      <c r="M22" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="N22" s="99"/>
-      <c r="O22" s="99"/>
-      <c r="P22" s="99"/>
-      <c r="Q22" s="131"/>
-      <c r="R22" s="169"/>
-      <c r="S22" s="170"/>
-      <c r="T22" s="101"/>
-      <c r="U22" s="102"/>
-      <c r="V22" s="102"/>
-      <c r="W22" s="100"/>
-      <c r="X22" s="174"/>
-      <c r="Y22" s="106"/>
-      <c r="Z22" s="107"/>
-      <c r="AA22" s="107"/>
+      <c r="N22" s="97"/>
+      <c r="O22" s="97"/>
+      <c r="P22" s="97"/>
+      <c r="Q22" s="129"/>
+      <c r="R22" s="187"/>
+      <c r="S22" s="188"/>
+      <c r="T22" s="99"/>
+      <c r="U22" s="100"/>
+      <c r="V22" s="100"/>
+      <c r="W22" s="98"/>
+      <c r="X22" s="192"/>
+      <c r="Y22" s="104"/>
+      <c r="Z22" s="105"/>
+      <c r="AA22" s="105"/>
       <c r="AB22" s="51"/>
       <c r="AC22" s="42"/>
       <c r="AD22" s="42"/>
@@ -4014,31 +4013,31 @@
       <c r="H23" s="35">
         <v>0</v>
       </c>
-      <c r="I23" s="96"/>
-      <c r="J23" s="98"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="108" t="s">
+      <c r="I23" s="94"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="M23" s="136"/>
-      <c r="N23" s="109" t="s">
+      <c r="M23" s="134"/>
+      <c r="N23" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="O23" s="109" t="s">
+      <c r="O23" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="P23" s="99"/>
-      <c r="Q23" s="131"/>
-      <c r="R23" s="169"/>
-      <c r="S23" s="170"/>
-      <c r="T23" s="101"/>
-      <c r="U23" s="102"/>
-      <c r="V23" s="102"/>
-      <c r="W23" s="100"/>
-      <c r="X23" s="174"/>
-      <c r="Y23" s="106"/>
-      <c r="Z23" s="107"/>
-      <c r="AA23" s="107"/>
+      <c r="P23" s="97"/>
+      <c r="Q23" s="129"/>
+      <c r="R23" s="187"/>
+      <c r="S23" s="188"/>
+      <c r="T23" s="99"/>
+      <c r="U23" s="100"/>
+      <c r="V23" s="100"/>
+      <c r="W23" s="98"/>
+      <c r="X23" s="192"/>
+      <c r="Y23" s="104"/>
+      <c r="Z23" s="105"/>
+      <c r="AA23" s="105"/>
       <c r="AB23" s="51"/>
       <c r="AC23" s="42"/>
       <c r="AD23" s="42"/>
@@ -4100,29 +4099,29 @@
       <c r="H24" s="35">
         <v>0</v>
       </c>
-      <c r="I24" s="96"/>
-      <c r="J24" s="98"/>
-      <c r="K24" s="98"/>
-      <c r="L24" s="98"/>
-      <c r="M24" s="99"/>
-      <c r="N24" s="136"/>
-      <c r="O24" s="97" t="s">
+      <c r="I24" s="94"/>
+      <c r="J24" s="96"/>
+      <c r="K24" s="96"/>
+      <c r="L24" s="96"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="134"/>
+      <c r="O24" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="P24" s="109" t="s">
+      <c r="P24" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="Q24" s="131"/>
-      <c r="R24" s="169"/>
-      <c r="S24" s="170"/>
-      <c r="T24" s="101"/>
-      <c r="U24" s="102"/>
-      <c r="V24" s="102"/>
-      <c r="W24" s="100"/>
-      <c r="X24" s="174"/>
-      <c r="Y24" s="106"/>
-      <c r="Z24" s="107"/>
-      <c r="AA24" s="107"/>
+      <c r="Q24" s="129"/>
+      <c r="R24" s="187"/>
+      <c r="S24" s="188"/>
+      <c r="T24" s="99"/>
+      <c r="U24" s="100"/>
+      <c r="V24" s="100"/>
+      <c r="W24" s="98"/>
+      <c r="X24" s="192"/>
+      <c r="Y24" s="104"/>
+      <c r="Z24" s="105"/>
+      <c r="AA24" s="105"/>
       <c r="AB24" s="51"/>
       <c r="AC24" s="42"/>
       <c r="AD24" s="42"/>
@@ -4161,7 +4160,7 @@
       <c r="BK24" s="42"/>
       <c r="BL24" s="30"/>
     </row>
-    <row r="25" spans="1:64" s="63" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1">
+    <row r="25" spans="1:64" s="62" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
       <c r="B25" s="60" t="s">
         <v>46</v>
@@ -4184,27 +4183,27 @@
       <c r="H25" s="35">
         <v>0</v>
       </c>
-      <c r="I25" s="96"/>
-      <c r="J25" s="98"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="98"/>
-      <c r="M25" s="99"/>
-      <c r="N25" s="108"/>
-      <c r="O25" s="108"/>
-      <c r="P25" s="136"/>
-      <c r="Q25" s="137" t="s">
+      <c r="I25" s="94"/>
+      <c r="J25" s="96"/>
+      <c r="K25" s="96"/>
+      <c r="L25" s="96"/>
+      <c r="M25" s="97"/>
+      <c r="N25" s="106"/>
+      <c r="O25" s="106"/>
+      <c r="P25" s="134"/>
+      <c r="Q25" s="135" t="s">
         <v>63</v>
       </c>
-      <c r="R25" s="169"/>
-      <c r="S25" s="170"/>
-      <c r="T25" s="101"/>
-      <c r="U25" s="102"/>
-      <c r="V25" s="102"/>
-      <c r="W25" s="100"/>
-      <c r="X25" s="174"/>
-      <c r="Y25" s="106"/>
-      <c r="Z25" s="107"/>
-      <c r="AA25" s="107"/>
+      <c r="R25" s="187"/>
+      <c r="S25" s="188"/>
+      <c r="T25" s="99"/>
+      <c r="U25" s="100"/>
+      <c r="V25" s="100"/>
+      <c r="W25" s="98"/>
+      <c r="X25" s="192"/>
+      <c r="Y25" s="104"/>
+      <c r="Z25" s="105"/>
+      <c r="AA25" s="105"/>
       <c r="AB25" s="51"/>
       <c r="AC25" s="42"/>
       <c r="AD25" s="42"/>
@@ -4266,28 +4265,28 @@
       <c r="H26" s="35">
         <v>0</v>
       </c>
-      <c r="I26" s="96"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="98"/>
-      <c r="M26" s="99"/>
-      <c r="N26" s="99"/>
-      <c r="O26" s="108"/>
-      <c r="P26" s="108"/>
-      <c r="R26" s="169"/>
-      <c r="S26" s="170"/>
-      <c r="T26" s="110" t="s">
+      <c r="I26" s="94"/>
+      <c r="J26" s="96"/>
+      <c r="K26" s="96"/>
+      <c r="L26" s="96"/>
+      <c r="M26" s="97"/>
+      <c r="N26" s="97"/>
+      <c r="O26" s="106"/>
+      <c r="P26" s="106"/>
+      <c r="R26" s="187"/>
+      <c r="S26" s="188"/>
+      <c r="T26" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="U26" s="151" t="s">
+      <c r="U26" s="149" t="s">
         <v>58</v>
       </c>
-      <c r="V26" s="102"/>
-      <c r="W26" s="100"/>
-      <c r="X26" s="174"/>
-      <c r="Y26" s="106"/>
-      <c r="Z26" s="107"/>
-      <c r="AA26" s="107"/>
+      <c r="V26" s="100"/>
+      <c r="W26" s="98"/>
+      <c r="X26" s="192"/>
+      <c r="Y26" s="104"/>
+      <c r="Z26" s="105"/>
+      <c r="AA26" s="105"/>
       <c r="AB26" s="51"/>
       <c r="AC26" s="42"/>
       <c r="AD26" s="42"/>
@@ -4335,36 +4334,36 @@
         <v>26</v>
       </c>
       <c r="D27" s="29"/>
-      <c r="E27" s="68">
+      <c r="E27" s="66">
         <v>45069</v>
       </c>
-      <c r="F27" s="68">
+      <c r="F27" s="66">
         <v>45072</v>
       </c>
-      <c r="G27" s="69">
+      <c r="G27" s="67">
         <f>SUM(G28:G31)</f>
         <v>6</v>
       </c>
       <c r="H27" s="29"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="85"/>
-      <c r="L27" s="85"/>
-      <c r="M27" s="85"/>
-      <c r="N27" s="85"/>
-      <c r="O27" s="85"/>
-      <c r="P27" s="85"/>
-      <c r="Q27" s="85"/>
-      <c r="R27" s="169"/>
-      <c r="S27" s="170"/>
-      <c r="T27" s="73"/>
-      <c r="U27" s="73"/>
-      <c r="V27" s="73"/>
-      <c r="W27" s="73"/>
-      <c r="X27" s="174"/>
-      <c r="Y27" s="73"/>
-      <c r="Z27" s="73"/>
-      <c r="AA27" s="111"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="83"/>
+      <c r="K27" s="83"/>
+      <c r="L27" s="83"/>
+      <c r="M27" s="83"/>
+      <c r="N27" s="83"/>
+      <c r="O27" s="83"/>
+      <c r="P27" s="83"/>
+      <c r="Q27" s="83"/>
+      <c r="R27" s="187"/>
+      <c r="S27" s="188"/>
+      <c r="T27" s="71"/>
+      <c r="U27" s="71"/>
+      <c r="V27" s="71"/>
+      <c r="W27" s="71"/>
+      <c r="X27" s="192"/>
+      <c r="Y27" s="71"/>
+      <c r="Z27" s="71"/>
+      <c r="AA27" s="109"/>
       <c r="AB27" s="41"/>
       <c r="AC27" s="41"/>
       <c r="AD27" s="41"/>
@@ -4426,29 +4425,29 @@
       <c r="H28" s="35">
         <v>0</v>
       </c>
-      <c r="I28" s="86"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="99"/>
-      <c r="N28" s="99"/>
-      <c r="O28" s="99"/>
-      <c r="P28" s="99"/>
-      <c r="Q28" s="90"/>
-      <c r="R28" s="169"/>
-      <c r="S28" s="170"/>
-      <c r="T28" s="138"/>
-      <c r="U28" s="139" t="s">
+      <c r="I28" s="84"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="97"/>
+      <c r="N28" s="97"/>
+      <c r="O28" s="97"/>
+      <c r="P28" s="97"/>
+      <c r="Q28" s="88"/>
+      <c r="R28" s="187"/>
+      <c r="S28" s="188"/>
+      <c r="T28" s="136"/>
+      <c r="U28" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="V28" s="139" t="s">
+      <c r="V28" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="W28" s="140"/>
-      <c r="X28" s="174"/>
-      <c r="Y28" s="94"/>
-      <c r="Z28" s="95"/>
-      <c r="AA28" s="95"/>
+      <c r="W28" s="138"/>
+      <c r="X28" s="192"/>
+      <c r="Y28" s="92"/>
+      <c r="Z28" s="93"/>
+      <c r="AA28" s="93"/>
       <c r="AB28" s="49"/>
       <c r="AC28" s="42"/>
       <c r="AD28" s="42"/>
@@ -4510,29 +4509,29 @@
       <c r="H29" s="35">
         <v>0</v>
       </c>
-      <c r="I29" s="96"/>
-      <c r="J29" s="98"/>
-      <c r="K29" s="98"/>
-      <c r="L29" s="98"/>
-      <c r="M29" s="99"/>
-      <c r="N29" s="99"/>
-      <c r="O29" s="99"/>
-      <c r="P29" s="99"/>
-      <c r="Q29" s="100"/>
-      <c r="R29" s="169"/>
-      <c r="S29" s="170"/>
-      <c r="T29" s="141"/>
-      <c r="U29" s="142"/>
-      <c r="V29" s="143" t="s">
+      <c r="I29" s="94"/>
+      <c r="J29" s="96"/>
+      <c r="K29" s="96"/>
+      <c r="L29" s="96"/>
+      <c r="M29" s="97"/>
+      <c r="N29" s="97"/>
+      <c r="O29" s="97"/>
+      <c r="P29" s="97"/>
+      <c r="Q29" s="98"/>
+      <c r="R29" s="187"/>
+      <c r="S29" s="188"/>
+      <c r="T29" s="139"/>
+      <c r="U29" s="140"/>
+      <c r="V29" s="141" t="s">
         <v>57</v>
       </c>
-      <c r="W29" s="144" t="s">
+      <c r="W29" s="142" t="s">
         <v>56</v>
       </c>
-      <c r="X29" s="174"/>
-      <c r="Y29" s="106"/>
-      <c r="Z29" s="107"/>
-      <c r="AA29" s="107"/>
+      <c r="X29" s="192"/>
+      <c r="Y29" s="104"/>
+      <c r="Z29" s="105"/>
+      <c r="AA29" s="105"/>
       <c r="AB29" s="50"/>
       <c r="AC29" s="42"/>
       <c r="AD29" s="42"/>
@@ -4594,27 +4593,27 @@
       <c r="H30" s="35">
         <v>0</v>
       </c>
-      <c r="I30" s="96"/>
-      <c r="J30" s="98"/>
-      <c r="K30" s="98"/>
-      <c r="L30" s="98"/>
-      <c r="M30" s="99"/>
-      <c r="N30" s="99"/>
-      <c r="O30" s="99"/>
-      <c r="P30" s="99"/>
-      <c r="Q30" s="90"/>
-      <c r="R30" s="169"/>
-      <c r="S30" s="170"/>
-      <c r="T30" s="145"/>
-      <c r="U30" s="142"/>
-      <c r="V30" s="146"/>
-      <c r="W30" s="144" t="s">
+      <c r="I30" s="94"/>
+      <c r="J30" s="96"/>
+      <c r="K30" s="96"/>
+      <c r="L30" s="96"/>
+      <c r="M30" s="97"/>
+      <c r="N30" s="97"/>
+      <c r="O30" s="97"/>
+      <c r="P30" s="97"/>
+      <c r="Q30" s="88"/>
+      <c r="R30" s="187"/>
+      <c r="S30" s="188"/>
+      <c r="T30" s="143"/>
+      <c r="U30" s="140"/>
+      <c r="V30" s="144"/>
+      <c r="W30" s="142" t="s">
         <v>57</v>
       </c>
-      <c r="X30" s="174"/>
-      <c r="Y30" s="106"/>
-      <c r="Z30" s="107"/>
-      <c r="AA30" s="107"/>
+      <c r="X30" s="192"/>
+      <c r="Y30" s="104"/>
+      <c r="Z30" s="105"/>
+      <c r="AA30" s="105"/>
       <c r="AB30" s="51"/>
       <c r="AC30" s="42"/>
       <c r="AD30" s="42"/>
@@ -4676,27 +4675,27 @@
       <c r="H31" s="35">
         <v>0</v>
       </c>
-      <c r="I31" s="96"/>
-      <c r="J31" s="98"/>
-      <c r="K31" s="98"/>
-      <c r="L31" s="98"/>
-      <c r="M31" s="99"/>
-      <c r="N31" s="99"/>
-      <c r="O31" s="99"/>
-      <c r="P31" s="99"/>
-      <c r="Q31" s="90"/>
-      <c r="R31" s="169"/>
-      <c r="S31" s="170"/>
-      <c r="T31" s="147"/>
-      <c r="U31" s="148"/>
-      <c r="V31" s="149"/>
-      <c r="W31" s="150" t="s">
+      <c r="I31" s="94"/>
+      <c r="J31" s="96"/>
+      <c r="K31" s="96"/>
+      <c r="L31" s="96"/>
+      <c r="M31" s="97"/>
+      <c r="N31" s="97"/>
+      <c r="O31" s="97"/>
+      <c r="P31" s="97"/>
+      <c r="Q31" s="88"/>
+      <c r="R31" s="187"/>
+      <c r="S31" s="188"/>
+      <c r="T31" s="145"/>
+      <c r="U31" s="146"/>
+      <c r="V31" s="147"/>
+      <c r="W31" s="148" t="s">
         <v>57</v>
       </c>
-      <c r="X31" s="174"/>
-      <c r="Y31" s="106"/>
-      <c r="Z31" s="107"/>
-      <c r="AA31" s="107"/>
+      <c r="X31" s="192"/>
+      <c r="Y31" s="104"/>
+      <c r="Z31" s="105"/>
+      <c r="AA31" s="105"/>
       <c r="AB31" s="51"/>
       <c r="AC31" s="42"/>
       <c r="AD31" s="42"/>
@@ -4744,36 +4743,36 @@
         <v>21</v>
       </c>
       <c r="D32" s="29"/>
-      <c r="E32" s="68">
+      <c r="E32" s="66">
         <v>45048</v>
       </c>
-      <c r="F32" s="68">
+      <c r="F32" s="66">
         <v>45079</v>
       </c>
-      <c r="G32" s="69">
+      <c r="G32" s="67">
         <f>SUM(G33:G36)</f>
         <v>19</v>
       </c>
       <c r="H32" s="29"/>
-      <c r="I32" s="84"/>
-      <c r="J32" s="85"/>
-      <c r="K32" s="85"/>
-      <c r="L32" s="85"/>
-      <c r="M32" s="85"/>
-      <c r="N32" s="85"/>
-      <c r="O32" s="85"/>
-      <c r="P32" s="85"/>
-      <c r="Q32" s="85"/>
-      <c r="R32" s="169"/>
-      <c r="S32" s="170"/>
-      <c r="T32" s="73"/>
-      <c r="U32" s="73"/>
-      <c r="V32" s="73"/>
-      <c r="W32" s="73"/>
-      <c r="X32" s="174"/>
-      <c r="Y32" s="73"/>
-      <c r="Z32" s="73"/>
-      <c r="AA32" s="111"/>
+      <c r="I32" s="82"/>
+      <c r="J32" s="83"/>
+      <c r="K32" s="83"/>
+      <c r="L32" s="83"/>
+      <c r="M32" s="83"/>
+      <c r="N32" s="83"/>
+      <c r="O32" s="83"/>
+      <c r="P32" s="83"/>
+      <c r="Q32" s="83"/>
+      <c r="R32" s="187"/>
+      <c r="S32" s="188"/>
+      <c r="T32" s="71"/>
+      <c r="U32" s="71"/>
+      <c r="V32" s="71"/>
+      <c r="W32" s="71"/>
+      <c r="X32" s="192"/>
+      <c r="Y32" s="71"/>
+      <c r="Z32" s="71"/>
+      <c r="AA32" s="109"/>
       <c r="AB32" s="51"/>
       <c r="AC32" s="42"/>
       <c r="AD32" s="42"/>
@@ -4835,27 +4834,27 @@
       <c r="H33" s="35">
         <v>0.8</v>
       </c>
-      <c r="I33" s="71" t="s">
+      <c r="I33" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="J33" s="88"/>
-      <c r="K33" s="88"/>
-      <c r="L33" s="88"/>
-      <c r="M33" s="89"/>
-      <c r="N33" s="89"/>
-      <c r="O33" s="89"/>
-      <c r="P33" s="89"/>
-      <c r="Q33" s="90"/>
-      <c r="R33" s="169"/>
-      <c r="S33" s="170"/>
-      <c r="T33" s="91"/>
-      <c r="U33" s="113"/>
-      <c r="V33" s="113"/>
-      <c r="W33" s="90"/>
-      <c r="X33" s="174"/>
-      <c r="Y33" s="94"/>
-      <c r="Z33" s="95"/>
-      <c r="AA33" s="95"/>
+      <c r="J33" s="86"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="87"/>
+      <c r="N33" s="87"/>
+      <c r="O33" s="87"/>
+      <c r="P33" s="87"/>
+      <c r="Q33" s="88"/>
+      <c r="R33" s="187"/>
+      <c r="S33" s="188"/>
+      <c r="T33" s="89"/>
+      <c r="U33" s="111"/>
+      <c r="V33" s="111"/>
+      <c r="W33" s="88"/>
+      <c r="X33" s="192"/>
+      <c r="Y33" s="92"/>
+      <c r="Z33" s="93"/>
+      <c r="AA33" s="93"/>
       <c r="AB33" s="51"/>
       <c r="AC33" s="42"/>
       <c r="AD33" s="42"/>
@@ -4917,49 +4916,49 @@
       <c r="H34" s="35">
         <v>0.03</v>
       </c>
-      <c r="I34" s="132"/>
-      <c r="J34" s="133"/>
-      <c r="K34" s="133"/>
-      <c r="L34" s="118" t="s">
+      <c r="I34" s="130"/>
+      <c r="J34" s="131"/>
+      <c r="K34" s="131"/>
+      <c r="L34" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="M34" s="120" t="s">
+      <c r="M34" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="N34" s="120" t="s">
+      <c r="N34" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="O34" s="120" t="s">
+      <c r="O34" s="118" t="s">
         <v>65</v>
       </c>
-      <c r="P34" s="120" t="s">
+      <c r="P34" s="118" t="s">
         <v>57</v>
       </c>
-      <c r="Q34" s="119" t="s">
+      <c r="Q34" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="R34" s="169"/>
-      <c r="S34" s="170"/>
-      <c r="T34" s="117" t="s">
+      <c r="R34" s="187"/>
+      <c r="S34" s="188"/>
+      <c r="T34" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="U34" s="118" t="s">
+      <c r="U34" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="V34" s="118" t="s">
+      <c r="V34" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="W34" s="119" t="s">
+      <c r="W34" s="117" t="s">
         <v>55</v>
       </c>
-      <c r="X34" s="174"/>
-      <c r="Y34" s="114" t="s">
+      <c r="X34" s="192"/>
+      <c r="Y34" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="Z34" s="115" t="s">
+      <c r="Z34" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="AA34" s="115" t="s">
+      <c r="AA34" s="113" t="s">
         <v>58</v>
       </c>
       <c r="AB34" s="51"/>
@@ -5023,27 +5022,27 @@
       <c r="H35" s="35">
         <v>1</v>
       </c>
-      <c r="I35" s="116" t="s">
+      <c r="I35" s="114" t="s">
         <v>56</v>
       </c>
-      <c r="J35" s="98"/>
-      <c r="K35" s="98"/>
-      <c r="L35" s="98"/>
-      <c r="M35" s="89"/>
-      <c r="N35" s="89"/>
-      <c r="O35" s="89"/>
-      <c r="P35" s="89"/>
-      <c r="Q35" s="90"/>
-      <c r="R35" s="169"/>
-      <c r="S35" s="170"/>
-      <c r="T35" s="101"/>
-      <c r="U35" s="102"/>
-      <c r="V35" s="102"/>
-      <c r="W35" s="100"/>
-      <c r="X35" s="174"/>
-      <c r="Y35" s="106"/>
-      <c r="Z35" s="107"/>
-      <c r="AA35" s="107"/>
+      <c r="J35" s="96"/>
+      <c r="K35" s="96"/>
+      <c r="L35" s="96"/>
+      <c r="M35" s="87"/>
+      <c r="N35" s="87"/>
+      <c r="O35" s="87"/>
+      <c r="P35" s="87"/>
+      <c r="Q35" s="88"/>
+      <c r="R35" s="187"/>
+      <c r="S35" s="188"/>
+      <c r="T35" s="99"/>
+      <c r="U35" s="100"/>
+      <c r="V35" s="100"/>
+      <c r="W35" s="98"/>
+      <c r="X35" s="192"/>
+      <c r="Y35" s="104"/>
+      <c r="Z35" s="105"/>
+      <c r="AA35" s="105"/>
       <c r="AB35" s="51"/>
       <c r="AC35" s="42"/>
       <c r="AD35" s="42"/>
@@ -5105,27 +5104,27 @@
       <c r="H36" s="36">
         <v>1</v>
       </c>
-      <c r="I36" s="116" t="s">
+      <c r="I36" s="114" t="s">
         <v>55</v>
       </c>
-      <c r="J36" s="98"/>
-      <c r="K36" s="98"/>
-      <c r="L36" s="98"/>
-      <c r="M36" s="89"/>
-      <c r="N36" s="89"/>
-      <c r="O36" s="89"/>
-      <c r="P36" s="89"/>
-      <c r="Q36" s="90"/>
-      <c r="R36" s="171"/>
-      <c r="S36" s="172"/>
-      <c r="T36" s="101"/>
-      <c r="U36" s="102"/>
-      <c r="V36" s="102"/>
-      <c r="W36" s="100"/>
-      <c r="X36" s="175"/>
-      <c r="Y36" s="106"/>
-      <c r="Z36" s="107"/>
-      <c r="AA36" s="107"/>
+      <c r="J36" s="96"/>
+      <c r="K36" s="96"/>
+      <c r="L36" s="96"/>
+      <c r="M36" s="87"/>
+      <c r="N36" s="87"/>
+      <c r="O36" s="87"/>
+      <c r="P36" s="87"/>
+      <c r="Q36" s="88"/>
+      <c r="R36" s="189"/>
+      <c r="S36" s="190"/>
+      <c r="T36" s="99"/>
+      <c r="U36" s="100"/>
+      <c r="V36" s="100"/>
+      <c r="W36" s="98"/>
+      <c r="X36" s="193"/>
+      <c r="Y36" s="104"/>
+      <c r="Z36" s="105"/>
+      <c r="AA36" s="105"/>
       <c r="AB36" s="51"/>
       <c r="AC36" s="42"/>
       <c r="AD36" s="42"/>
@@ -5166,7 +5165,7 @@
     </row>
     <row r="37" spans="1:64" ht="21" customHeight="1">
       <c r="A37" s="20"/>
-      <c r="I37" s="70"/>
+      <c r="I37" s="68"/>
       <c r="AB37" s="41"/>
       <c r="AC37" s="41"/>
       <c r="AD37" s="41"/>
@@ -5327,7 +5326,7 @@
     </row>
     <row r="41" spans="1:64" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="AA41" s="203"/>
+      <c r="AA41" s="165"/>
       <c r="AB41" s="51"/>
       <c r="AC41" s="42"/>
       <c r="AD41" s="42"/>
@@ -5565,7 +5564,25 @@
       <c r="BL44" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R11:S36"/>
+    <mergeCell ref="X11:X36"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="BB9:BF9"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="X9:AA9"/>
+    <mergeCell ref="I8:AA8"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="BG9:BK9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="AW8:BK8"/>
+    <mergeCell ref="AH8:AV8"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AH9:AL9"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="L9:O9"/>
     <mergeCell ref="P9:S9"/>
@@ -5582,23 +5599,6 @@
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="E8:E10"/>
-    <mergeCell ref="BG9:BK9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="AW8:BK8"/>
-    <mergeCell ref="AH8:AV8"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="R11:S36"/>
-    <mergeCell ref="X11:X36"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="BB9:BF9"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="X9:AA9"/>
-    <mergeCell ref="I8:AA8"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="I9:K9"/>
   </mergeCells>
   <conditionalFormatting sqref="H17:H36 H12:H15">
     <cfRule type="colorScale" priority="13">

</xml_diff>